<commit_message>
feat: update AEFI for DHIS2v 2.33, 2.34, 2.35
</commit_message>
<xml_diff>
--- a/metadata/AEFI/AEFI_TRACKER_V1_DHIS2.33/reference.xlsx
+++ b/metadata/AEFI/AEFI_TRACKER_V1_DHIS2.33/reference.xlsx
@@ -447,7 +447,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="69.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,7 +479,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>AEFI</v>
+        <v>V1.1.2</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>TRACKER</v>
+        <v>DHIS2.33.8-3c90b70</v>
       </c>
     </row>
     <row r="6">
@@ -495,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>V1.1.0</v>
+        <v>20210406T115721</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>AEFI_TRACKER_AEFI_TRACKER_V1.1.0_DHIS2.33.8-3c90b70_20210318T130229</v>
+        <v>AEFI_TRACKER_V1.1.2_DHIS2.33.8-3c90b70_20210406T115721</v>
       </c>
     </row>
   </sheetData>
@@ -580,7 +580,7 @@
         <v>PmqH3jmR0a3</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>sB1IHYu2xQT</v>
+        <v>First Name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>sB1IHYu2xQT</v>
@@ -597,7 +597,7 @@
         <v>k77IMif2vZN</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>ENRjVGxVL6l</v>
+        <v>Surname</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>ENRjVGxVL6l</v>
@@ -614,7 +614,7 @@
         <v>xqb0WbHJcwg</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>NI0QRzJvQ0k</v>
+        <v>Date of birth</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>NI0QRzJvQ0k</v>
@@ -631,7 +631,7 @@
         <v>G6EB7Mvdtz2</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>oindugucx72</v>
+        <v>Sex</v>
       </c>
       <c r="C7" s="5" t="str">
         <v>oindugucx72</v>
@@ -648,7 +648,7 @@
         <v>B3GhkhHeteN</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Xhdn49gUd52</v>
+        <v>Home Address</v>
       </c>
       <c r="C8" s="4" t="str">
         <v>Xhdn49gUd52</v>
@@ -683,7 +683,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G138"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -3713,10 +3713,10 @@
     </row>
     <row r="132">
       <c r="A132" s="4" t="str">
-        <v>AEFI AEFI - Bell's Palsy</v>
+        <v>AEFI - Fever &gt; or equal to 38 degrees C</v>
       </c>
       <c r="B132" s="4" t="str">
-        <v>Bell's Palsy</v>
+        <v>Fever &gt; or equal to 38 degrees C</v>
       </c>
       <c r="C132" s="4" t="str">
         <v/>
@@ -3731,21 +3731,21 @@
         <v/>
       </c>
       <c r="G132" s="4" t="str">
-        <v>PuCFugChuxx</v>
+        <v>LbT5aALwcOj</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="5" t="str">
-        <v>AEFI - Fever &gt; or equal to 38 degrees C</v>
+        <v>AEFI - Investigation date</v>
       </c>
       <c r="B133" s="5" t="str">
-        <v>Fever &gt; or equal to 38 degrees C</v>
+        <v>Investigation date</v>
       </c>
       <c r="C133" s="5" t="str">
         <v/>
       </c>
       <c r="D133" s="5" t="str">
-        <v/>
+        <v>Date when detailed investigation (including field investigation) was done</v>
       </c>
       <c r="E133" s="5" t="str">
         <v>default</v>
@@ -3754,21 +3754,21 @@
         <v/>
       </c>
       <c r="G133" s="5" t="str">
-        <v>LbT5aALwcOj</v>
+        <v>yUBUbMo3kGv</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="4" t="str">
-        <v>AEFI - Investigation date</v>
+        <v>AEFI - Other AEFI</v>
       </c>
       <c r="B134" s="4" t="str">
-        <v>Investigation date</v>
+        <v>AEFI Other AEFI</v>
       </c>
       <c r="C134" s="4" t="str">
         <v/>
       </c>
       <c r="D134" s="4" t="str">
-        <v>Date when detailed investigation (including field investigation) was done</v>
+        <v>Whether other side effect was reported by client</v>
       </c>
       <c r="E134" s="4" t="str">
         <v>default</v>
@@ -3777,21 +3777,21 @@
         <v/>
       </c>
       <c r="G134" s="4" t="str">
-        <v>yUBUbMo3kGv</v>
+        <v>GfnOHMNK1BH</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="5" t="str">
-        <v>AEFI -  Lymphadenopathy</v>
+        <v>AEFI - Other AEFI Date</v>
       </c>
       <c r="B135" s="5" t="str">
-        <v>Lymphadenopathy</v>
+        <v>AEFI Other AEFI date</v>
       </c>
       <c r="C135" s="5" t="str">
-        <v/>
+        <v>se_other_date</v>
       </c>
       <c r="D135" s="5" t="str">
-        <v/>
+        <v>Date other side effects were experienced by client</v>
       </c>
       <c r="E135" s="5" t="str">
         <v>default</v>
@@ -3800,21 +3800,21 @@
         <v/>
       </c>
       <c r="G135" s="5" t="str">
-        <v>S1hrcFVHKoh</v>
+        <v>BeSHubSs97e</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="4" t="str">
-        <v>AEFI - Other AEFI</v>
+        <v>AEFI - Vaccine name</v>
       </c>
       <c r="B136" s="4" t="str">
-        <v>AEFI Other AEFI</v>
+        <v>Vaccine name</v>
       </c>
       <c r="C136" s="4" t="str">
         <v/>
       </c>
       <c r="D136" s="4" t="str">
-        <v>Whether other side effect was reported by client</v>
+        <v xml:space="preserve">The vaccine that is suspected to have caused the AEFI (provide brand name, if possible) </v>
       </c>
       <c r="E136" s="4" t="str">
         <v>default</v>
@@ -3823,52 +3823,6 @@
         <v/>
       </c>
       <c r="G136" s="4" t="str">
-        <v>GfnOHMNK1BH</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="5" t="str">
-        <v>AEFI - Other AEFI Date</v>
-      </c>
-      <c r="B137" s="5" t="str">
-        <v>AEFI Other AEFI date</v>
-      </c>
-      <c r="C137" s="5" t="str">
-        <v>se_other_date</v>
-      </c>
-      <c r="D137" s="5" t="str">
-        <v>Date other side effects were experienced by client</v>
-      </c>
-      <c r="E137" s="5" t="str">
-        <v>default</v>
-      </c>
-      <c r="F137" s="5" t="str">
-        <v/>
-      </c>
-      <c r="G137" s="5" t="str">
-        <v>BeSHubSs97e</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="4" t="str">
-        <v>AEFI - Vaccine name</v>
-      </c>
-      <c r="B138" s="4" t="str">
-        <v>Vaccine name</v>
-      </c>
-      <c r="C138" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D138" s="4" t="str">
-        <v xml:space="preserve">The vaccine that is suspected to have caused the AEFI (provide brand name, if possible) </v>
-      </c>
-      <c r="E138" s="4" t="str">
-        <v>default</v>
-      </c>
-      <c r="F138" s="4" t="str">
-        <v/>
-      </c>
-      <c r="G138" s="4" t="str">
         <v>u6OlTToQfhr</v>
       </c>
     </row>
@@ -3878,13 +3832,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B153"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3900,7 +3854,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>AEFI - Other vaccine 1 name</v>
+        <v>AEFI - Batch/lot number (Vaccine 1)</v>
       </c>
     </row>
     <row r="3">
@@ -3908,7 +3862,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>AEFI - Severe event reported</v>
+        <v>AEFI - Diluent batch/lot number 4</v>
       </c>
     </row>
     <row r="4">
@@ -3916,7 +3870,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>AEFI - Muscle pain</v>
+        <v>AEFI - Vaccine 4 name</v>
       </c>
     </row>
     <row r="5">
@@ -3924,7 +3878,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>AEFI - Drowsiness</v>
+        <v>AEFI - Tiredness</v>
       </c>
     </row>
     <row r="6">
@@ -3932,7 +3886,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v xml:space="preserve">AEFI - Specify (Final causality - Unclassifiable) </v>
+        <v>AEFI - Vaccine 2 dose</v>
       </c>
     </row>
     <row r="7">
@@ -3940,7 +3894,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>AEFI - Injection site soreness</v>
+        <v>AEFI - Batch/lot number (Vaccine 2)</v>
       </c>
     </row>
     <row r="8">
@@ -3948,7 +3902,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>AEFI - Skin rash</v>
+        <v>AEFI - Autopsy conducted</v>
       </c>
     </row>
     <row r="9">
@@ -3956,7 +3910,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>AEFI - Sepsis</v>
+        <v>AEFI - Pregnancy stage (Trimester)</v>
       </c>
     </row>
     <row r="10">
@@ -3964,7 +3918,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 4)</v>
+        <v>AEFI - Reconstitution time 1</v>
       </c>
     </row>
     <row r="11">
@@ -3972,7 +3926,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>AEFI - Vaccine 4 name</v>
+        <v>AEFI - Headache</v>
       </c>
     </row>
     <row r="12">
@@ -3980,7 +3934,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>AEFI - Vaccine 4 brand</v>
+        <v>AEFI - Contact number</v>
       </c>
     </row>
     <row r="13">
@@ -3988,7 +3942,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>AEFI - Vaccine 2 brand</v>
+        <v>AEFI - Other diluent 4 name</v>
       </c>
     </row>
     <row r="14">
@@ -3996,7 +3950,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>AEFI - Severe local reaction</v>
+        <v>AEFI - Expiry date (Vaccine 3)</v>
       </c>
     </row>
     <row r="15">
@@ -4004,7 +3958,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>AEFI AEFI - Bell's Palsy</v>
+        <v>AEFI - Fever</v>
       </c>
     </row>
     <row r="16">
@@ -4012,7 +3966,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>AEFI - Vaccine 3 name</v>
+        <v>AEFI - Other Signs and symptoms</v>
       </c>
     </row>
     <row r="17">
@@ -4020,7 +3974,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>AEFI - Reconstitution date 4</v>
+        <v>AEFI - Is the patient pregnant?</v>
       </c>
     </row>
     <row r="18">
@@ -4028,7 +3982,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>AEFI - Vaccination 2 time</v>
+        <v>AEFI - Diarrhoea</v>
       </c>
     </row>
     <row r="19">
@@ -4036,7 +3990,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>AEFI - Other diluent 2 name</v>
+        <v>AEFI - Persistent or significant disability</v>
       </c>
     </row>
     <row r="20">
@@ -4044,7 +3998,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>AEFI - Date of death</v>
+        <v>AEFI - Skin rash</v>
       </c>
     </row>
     <row r="21">
@@ -4052,7 +4006,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>AEFI - Vaccine 1 dose</v>
+        <v>AEFI - Lymphadenopathy</v>
       </c>
     </row>
     <row r="22">
@@ -4060,7 +4014,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>AEFI - Contact number</v>
+        <v>AEFI - Bell's Palsy</v>
       </c>
     </row>
     <row r="23">
@@ -4068,7 +4022,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>AEFI - Persistent crying</v>
+        <v>AEFI - Reconstitution time 4</v>
       </c>
     </row>
     <row r="24">
@@ -4084,7 +4038,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>AEFI - Nausea</v>
+        <v>AEFI - Date of death</v>
       </c>
     </row>
     <row r="26">
@@ -4092,7 +4046,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>AEFI - Diluent 4</v>
+        <v>AEFI - Vaccine 1 name</v>
       </c>
     </row>
     <row r="27">
@@ -4100,7 +4054,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>AEFI - Anaphylaxis</v>
+        <v>AEFI - Valid Diagnosis</v>
       </c>
     </row>
     <row r="28">
@@ -4108,7 +4062,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>AEFI - Vaccination 3 date</v>
+        <v>AEFI - Expiry date (Vaccine 2)</v>
       </c>
     </row>
     <row r="29">
@@ -4116,7 +4070,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>AEFI - Diluent batch/lot number 1</v>
+        <v>AEFI - Vaccination 4 date</v>
       </c>
     </row>
     <row r="30">
@@ -4124,7 +4078,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>AEFI - Valid Diagnosis</v>
+        <v>AEFI - Reconstitution date 3</v>
       </c>
     </row>
     <row r="31">
@@ -4132,7 +4086,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>AEFI - Fainting</v>
+        <v>AEFI - Vaccination 4 time</v>
       </c>
     </row>
     <row r="32">
@@ -4140,7 +4094,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>AEFI - Expiry date (Vaccine 1)</v>
+        <v>AEFI - Thrombocytopenia</v>
       </c>
     </row>
     <row r="33">
@@ -4148,7 +4102,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>AEFI - Diluent 1</v>
+        <v>AEFI - Seizure type</v>
       </c>
     </row>
     <row r="34">
@@ -4156,7 +4110,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>AEFI - Abscess</v>
+        <v>AEFI - Batch/lot number (Vaccine 4)</v>
       </c>
     </row>
     <row r="35">
@@ -4164,7 +4118,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>AEFI - Diluent 3</v>
+        <v>AEFI - Vomiting</v>
       </c>
     </row>
     <row r="36">
@@ -4172,7 +4126,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>AEFI - Other vaccine 3 name</v>
+        <v>AEFI - Other vaccine 1 name</v>
       </c>
     </row>
     <row r="37">
@@ -4180,7 +4134,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>AEFI - Mild fever</v>
+        <v>AEFI - Vaccine 2 name</v>
       </c>
     </row>
     <row r="38">
@@ -4188,7 +4142,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>AEFI - Sore throat</v>
+        <v>AEFI - Date of final classification</v>
       </c>
     </row>
     <row r="39">
@@ -4196,7 +4150,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>AEFI - Thrombocytopenia</v>
+        <v>AEFI - Muscle pain</v>
       </c>
     </row>
     <row r="40">
@@ -4204,7 +4158,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>AEFI - Vaccine 4 dose</v>
+        <v>AEFI - Reconstitution date 2</v>
       </c>
     </row>
     <row r="41">
@@ -4212,7 +4166,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>AEFI - Medical history</v>
+        <v>AEFI - Investigation needed</v>
       </c>
     </row>
     <row r="42">
@@ -4220,7 +4174,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>AEFI - Final causality assessment sub-classification</v>
+        <v>AEFI - Diluent batch/lot number 3</v>
       </c>
     </row>
     <row r="43">
@@ -4228,7 +4182,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>AEFI - Reconstitution date 2</v>
+        <v>AEFI - Investigation planned date</v>
       </c>
     </row>
     <row r="44">
@@ -4236,7 +4190,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>AEFI - Lymph node enlargement</v>
+        <v>AEFI - Vaccine name</v>
       </c>
     </row>
     <row r="45">
@@ -4244,7 +4198,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>AEFI - Other AEFI Date</v>
+        <v>AEFI - Abdominal pain</v>
       </c>
     </row>
     <row r="46">
@@ -4252,7 +4206,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>AEFI - Dizziness</v>
+        <v>AEFI - Final causality assessment classification</v>
       </c>
     </row>
     <row r="47">
@@ -4260,7 +4214,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>AEFI - Is the patient pregnant?</v>
+        <v>AEFI - Reconstitution time 3</v>
       </c>
     </row>
     <row r="48">
@@ -4268,7 +4222,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>AEFI - Vaccination 2 date</v>
+        <v>AEFI - Abscess</v>
       </c>
     </row>
     <row r="49">
@@ -4276,7 +4230,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>AEFI - Date when seen for approval at national level</v>
+        <v>AEFI - Congenital anomaly</v>
       </c>
     </row>
     <row r="50">
@@ -4284,7 +4238,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>AEFI - Severe local reaction &gt; 3 days</v>
+        <v>AEFI - Injection site tenderness</v>
       </c>
     </row>
     <row r="51">
@@ -4292,7 +4246,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>AEFI - Loss of apetite</v>
+        <v>AEFI - Medical history</v>
       </c>
     </row>
     <row r="52">
@@ -4300,7 +4254,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v>AEFI - Comments</v>
+        <v>AEFI - Lymph node enlargement</v>
       </c>
     </row>
     <row r="53">
@@ -4308,7 +4262,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>AEFI - Reconstitution time 1</v>
+        <v>AEFI - Specify other (Severe event)</v>
       </c>
     </row>
     <row r="54">
@@ -4316,7 +4270,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>AEFI - Vaccine 1 brand</v>
+        <v>AEFI - Reconstitution time 2</v>
       </c>
     </row>
     <row r="55">
@@ -4324,7 +4278,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>AEFI - Life threatening</v>
+        <v>AEFI - Chills</v>
       </c>
     </row>
     <row r="56">
@@ -4332,7 +4286,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B56" s="4" t="str">
-        <v>AEFI - Diluent batch/lot number 4</v>
+        <v>AEFI - Reconstitution date 1</v>
       </c>
     </row>
     <row r="57">
@@ -4340,7 +4294,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>AEFI - Batch/lot number (Vaccine 3)</v>
+        <v>AEFI - Reporter of AEFI case</v>
       </c>
     </row>
     <row r="58">
@@ -4348,7 +4302,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B58" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 1)</v>
+        <v>AEFI - AEFI start date</v>
       </c>
     </row>
     <row r="59">
@@ -4356,7 +4310,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>AEFI - Vaccination 1 time</v>
+        <v>AEFI - Severe local reaction &gt; 3 days</v>
       </c>
     </row>
     <row r="60">
@@ -4364,7 +4318,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B60" s="4" t="str">
-        <v>AEFI - Specify other (Adverse event)</v>
+        <v>AEFI - Death</v>
       </c>
     </row>
     <row r="61">
@@ -4372,7 +4326,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v>AEFI - Encephalopathy</v>
+        <v>AEFI - Vaccination 3 date</v>
       </c>
     </row>
     <row r="62">
@@ -4380,7 +4334,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B62" s="4" t="str">
-        <v>AEFI - Congenital anomaly</v>
+        <v>AEFI - Specify other (Adverse event)</v>
       </c>
     </row>
     <row r="63">
@@ -4388,7 +4342,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B63" s="5" t="str">
-        <v>AEFI - Date of final classification</v>
+        <v>AEFI - Vaccine 3 dose</v>
       </c>
     </row>
     <row r="64">
@@ -4396,7 +4350,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B64" s="4" t="str">
-        <v>AEFI - Vomiting</v>
+        <v>AEFI - Vaccination 2 date</v>
       </c>
     </row>
     <row r="65">
@@ -4404,7 +4358,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B65" s="5" t="str">
-        <v>AEFI - Reconstitution date 3</v>
+        <v>AEFI - AEFI outcome</v>
       </c>
     </row>
     <row r="66">
@@ -4412,7 +4366,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B66" s="4" t="str">
-        <v>AEFI - Hospitalization</v>
+        <v>AEFI - AEFI time</v>
       </c>
     </row>
     <row r="67">
@@ -4420,7 +4374,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B67" s="5" t="str">
-        <v>AEFI - Vaccination 4 time</v>
+        <v>AEFI - Diluent batch/lot number 2</v>
       </c>
     </row>
     <row r="68">
@@ -4428,7 +4382,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B68" s="4" t="str">
-        <v>AEFI - Bell's Palsy</v>
+        <v>AEFI - Vaccine 1 dose</v>
       </c>
     </row>
     <row r="69">
@@ -4436,7 +4390,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B69" s="5" t="str">
-        <v>AEFI - Vaccine 2 name</v>
+        <v>AEFI - Vaccine 3 name</v>
       </c>
     </row>
     <row r="70">
@@ -4444,7 +4398,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B70" s="4" t="str">
-        <v>AEFI - Expiry date (Vaccine 3)</v>
+        <v>AEFI - Mild fever</v>
       </c>
     </row>
     <row r="71">
@@ -4452,7 +4406,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B71" s="5" t="str">
-        <v>AEFI - Injection site tenderness</v>
+        <v>AEFI - Batch/lot number (Vaccine 3)</v>
       </c>
     </row>
     <row r="72">
@@ -4460,7 +4414,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B72" s="4" t="str">
-        <v>AEFI - Other vaccine 4 name</v>
+        <v>AEFI - E-mail address</v>
       </c>
     </row>
     <row r="73">
@@ -4468,7 +4422,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B73" s="5" t="str">
-        <v>AEFI - Diluent batch/lot number 3</v>
+        <v>AEFI - Expiry date (Diluent 4)</v>
       </c>
     </row>
     <row r="74">
@@ -4476,7 +4430,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B74" s="4" t="str">
-        <v>AEFI -  Lymphadenopathy</v>
+        <v>AEFI - Vaccine 1 brand</v>
       </c>
     </row>
     <row r="75">
@@ -4484,7 +4438,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>AEFI - Expiry date (Vaccine 2)</v>
+        <v>AEFI - Itching</v>
       </c>
     </row>
     <row r="76">
@@ -4492,7 +4446,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B76" s="4" t="str">
-        <v>AEFI - Poor breast feeding</v>
+        <v>AEFI - Joint pain</v>
       </c>
     </row>
     <row r="77">
@@ -4500,7 +4454,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B77" s="5" t="str">
-        <v>AEFI - Nasal congestion</v>
+        <v>AEFI - Expiry date (Vaccine 4)</v>
       </c>
     </row>
     <row r="78">
@@ -4508,7 +4462,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B78" s="4" t="str">
-        <v>AEFI - Vaccination 3 time</v>
+        <v>AEFI - Severe event reported</v>
       </c>
     </row>
     <row r="79">
@@ -4516,7 +4470,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>AEFI - Irritability</v>
+        <v>AEFI - Vaccination 1 date</v>
       </c>
     </row>
     <row r="80">
@@ -4524,7 +4478,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B80" s="4" t="str">
-        <v>AEFI - AEFI start date</v>
+        <v>AEFI - Position/Department</v>
       </c>
     </row>
     <row r="81">
@@ -4532,7 +4486,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B81" s="5" t="str">
-        <v>AEFI - Cough</v>
+        <v>AEFI - Other diluent 2 name</v>
       </c>
     </row>
     <row r="82">
@@ -4540,7 +4494,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B82" s="4" t="str">
-        <v>AEFI - Vaccine 2 dose</v>
+        <v>AEFI - Other diluent 1 name</v>
       </c>
     </row>
     <row r="83">
@@ -4548,7 +4502,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B83" s="5" t="str">
-        <v>AEFI - Pregnancy stage (Trimester)</v>
+        <v>AEFI - Nausea</v>
       </c>
     </row>
     <row r="84">
@@ -4556,7 +4510,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B84" s="4" t="str">
-        <v>AEFI - Diarrhoea</v>
+        <v xml:space="preserve">AEFI - Specify (Final causality - Unclassifiable) </v>
       </c>
     </row>
     <row r="85">
@@ -4564,7 +4518,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B85" s="5" t="str">
-        <v>AEFI - E-mail address</v>
+        <v>AEFI - Poor breast feeding</v>
       </c>
     </row>
     <row r="86">
@@ -4572,7 +4526,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B86" s="4" t="str">
-        <v>AEFI - Joint pain</v>
+        <v>AEFI - Vaccination 1 time</v>
       </c>
     </row>
     <row r="87">
@@ -4580,7 +4534,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B87" s="5" t="str">
-        <v>AEFI - Other (Severe event)</v>
+        <v>AEFI - Reconstitution date 4</v>
       </c>
     </row>
     <row r="88">
@@ -4588,7 +4542,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B88" s="4" t="str">
-        <v>AEFI - Reconstitution time 4</v>
+        <v>AEFI - Other AEFI</v>
       </c>
     </row>
     <row r="89">
@@ -4596,7 +4550,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B89" s="5" t="str">
-        <v>AEFI - AEFI outcome</v>
+        <v>AEFI - Irritability</v>
       </c>
     </row>
     <row r="90">
@@ -4604,7 +4558,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B90" s="4" t="str">
-        <v>AEFI - Reporter of AEFI case</v>
+        <v>AEFI - Other vaccine 2 name</v>
       </c>
     </row>
     <row r="91">
@@ -4612,7 +4566,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B91" s="5" t="str">
-        <v>AEFI - Abdominal pain</v>
+        <v>AEFI - Nasal congestion</v>
       </c>
     </row>
     <row r="92">
@@ -4620,7 +4574,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B92" s="4" t="str">
-        <v>AEFI - Seizures</v>
+        <v>AEFI - Comments</v>
       </c>
     </row>
     <row r="93">
@@ -4628,7 +4582,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B93" s="5" t="str">
-        <v>AEFI - Diluent batch/lot number 2</v>
+        <v>AEFI - Persistent crying</v>
       </c>
     </row>
     <row r="94">
@@ -4636,7 +4590,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B94" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 3)</v>
+        <v>AEFI - Diluent 3</v>
       </c>
     </row>
     <row r="95">
@@ -4644,7 +4598,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B95" s="5" t="str">
-        <v>AEFI - Batch/lot number (Vaccine 4)</v>
+        <v>AEFI - Other diluent 3 name</v>
       </c>
     </row>
     <row r="96">
@@ -4652,7 +4606,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B96" s="4" t="str">
-        <v>AEFI - Expiry date (Vaccine 4)</v>
+        <v>AEFI - Reporter's address</v>
       </c>
     </row>
     <row r="97">
@@ -4660,7 +4614,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B97" s="5" t="str">
-        <v>AEFI - Death</v>
+        <v>AEFI - Vaccine 4 brand</v>
       </c>
     </row>
     <row r="98">
@@ -4668,7 +4622,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B98" s="4" t="str">
-        <v>AEFI - Severe local reaction beyond nearest joint</v>
+        <v>AEFI - Diluent 1</v>
       </c>
     </row>
     <row r="99">
@@ -4676,7 +4630,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B99" s="5" t="str">
-        <v>AEFI - Autopsy conducted</v>
+        <v>AEFI - Dizziness</v>
       </c>
     </row>
     <row r="100">
@@ -4684,7 +4638,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B100" s="4" t="str">
-        <v>AEFI - Reconstitution time 3</v>
+        <v>AEFI - Injection site soreness</v>
       </c>
     </row>
     <row r="101">
@@ -4692,7 +4646,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>AEFI - Reconstitution time 2</v>
+        <v>AEFI - Fatigue</v>
       </c>
     </row>
     <row r="102">
@@ -4700,7 +4654,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B102" s="4" t="str">
-        <v>AEFI - AEFI time</v>
+        <v>AEFI - Vaccination 2 time</v>
       </c>
     </row>
     <row r="103">
@@ -4708,7 +4662,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B103" s="5" t="str">
-        <v>AEFI - Toxic shock syndrome</v>
+        <v>AEFI - Seizures</v>
       </c>
     </row>
     <row r="104">
@@ -4716,7 +4670,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B104" s="4" t="str">
-        <v>AEFI - Other vaccine 2 name</v>
+        <v>AEFI - Diluent 4</v>
       </c>
     </row>
     <row r="105">
@@ -4724,7 +4678,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B105" s="5" t="str">
-        <v>AEFI - Persistent or significant disability</v>
+        <v>AEFI - Other vaccine 4 name</v>
       </c>
     </row>
     <row r="106">
@@ -4732,7 +4686,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B106" s="4" t="str">
-        <v>AEFI - Itching</v>
+        <v>AEFI - Severe local reaction beyond nearest joint</v>
       </c>
     </row>
     <row r="107">
@@ -4740,7 +4694,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B107" s="5" t="str">
-        <v>AEFI - Chills</v>
+        <v>AEFI - Is the patient lactating?</v>
       </c>
     </row>
     <row r="108">
@@ -4748,7 +4702,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B108" s="4" t="str">
-        <v>AEFI - Lymphadenopathy</v>
+        <v>AEFI - Date when seen for approval at national level</v>
       </c>
     </row>
     <row r="109">
@@ -4756,7 +4710,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B109" s="5" t="str">
-        <v>AEFI - Is the patient lactating?</v>
+        <v>AEFI - Diluent batch/lot number 1</v>
       </c>
     </row>
     <row r="110">
@@ -4764,7 +4718,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B110" s="4" t="str">
-        <v>AEFI - Tiredness</v>
+        <v>AEFI - Sepsis</v>
       </c>
     </row>
     <row r="111">
@@ -4772,7 +4726,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B111" s="5" t="str">
-        <v>AEFI - Reconstitution date 1</v>
+        <v>AEFI - Vaccination 3 time</v>
       </c>
     </row>
     <row r="112">
@@ -4780,7 +4734,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B112" s="4" t="str">
-        <v>AEFI - Other diluent 3 name</v>
+        <v>AEFI - Other vaccine 3 name</v>
       </c>
     </row>
     <row r="113">
@@ -4788,7 +4742,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B113" s="5" t="str">
-        <v>AEFI - Investigation planned date</v>
+        <v>AEFI - Expiry date (Diluent 3)</v>
       </c>
     </row>
     <row r="114">
@@ -4796,7 +4750,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B114" s="4" t="str">
-        <v>AEFI - Position/Department</v>
+        <v>AEFI - Fainting</v>
       </c>
     </row>
     <row r="115">
@@ -4804,7 +4758,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B115" s="5" t="str">
-        <v>AEFI - Final causality assessment classification</v>
+        <v>AEFI - Anaphylaxis</v>
       </c>
     </row>
     <row r="116">
@@ -4812,7 +4766,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B116" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 2)</v>
+        <v>AEFI - Diluent 2</v>
       </c>
     </row>
     <row r="117">
@@ -4820,7 +4774,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B117" s="5" t="str">
-        <v>AEFI - Vaccination 1 date</v>
+        <v>AEFI - Hospitalization</v>
       </c>
     </row>
     <row r="118">
@@ -4828,7 +4782,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B118" s="4" t="str">
-        <v>AEFI - Vaccine 1 name</v>
+        <v>AEFI - Expiry date (Diluent 2)</v>
       </c>
     </row>
     <row r="119">
@@ -4836,7 +4790,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B119" s="5" t="str">
-        <v>AEFI - Diluent 2</v>
+        <v>AEFI - Final causality assessment sub-classification</v>
       </c>
     </row>
     <row r="120">
@@ -4844,7 +4798,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B120" s="4" t="str">
-        <v>AEFI - Other diluent 1 name</v>
+        <v>AEFI - Vaccine 2 brand</v>
       </c>
     </row>
     <row r="121">
@@ -4852,7 +4806,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B121" s="5" t="str">
-        <v>AEFI - Other Signs and symptoms</v>
+        <v>AEFI - Life threatening</v>
       </c>
     </row>
     <row r="122">
@@ -4860,7 +4814,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B122" s="4" t="str">
-        <v>AEFI - Vaccine name</v>
+        <v>AEFI - Vaccine 3 brand</v>
       </c>
     </row>
     <row r="123">
@@ -4868,7 +4822,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B123" s="5" t="str">
-        <v>AEFI - Headache</v>
+        <v>AEFI - Vaccine 4 dose</v>
       </c>
     </row>
     <row r="124">
@@ -4876,7 +4830,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B124" s="4" t="str">
-        <v>AEFI - Specify other (Severe event)</v>
+        <v>AEFI - Toxic shock syndrome</v>
       </c>
     </row>
     <row r="125">
@@ -4884,7 +4838,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B125" s="5" t="str">
-        <v>AEFI - Fatigue</v>
+        <v>AEFI - Encephalopathy</v>
       </c>
     </row>
     <row r="126">
@@ -4892,7 +4846,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B126" s="4" t="str">
-        <v>AEFI - Vaccine 3 brand</v>
+        <v>AEFI - Expiry date (Diluent 1)</v>
       </c>
     </row>
     <row r="127">
@@ -4900,7 +4854,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B127" s="5" t="str">
-        <v>AEFI - Vaccine 3 dose</v>
+        <v>AEFI - Expiry date (Vaccine 1)</v>
       </c>
     </row>
     <row r="128">
@@ -4908,7 +4862,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B128" s="4" t="str">
-        <v>AEFI - Other AEFI</v>
+        <v>AEFI - Severe local reaction</v>
       </c>
     </row>
     <row r="129">
@@ -4916,7 +4870,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B129" s="5" t="str">
-        <v>AEFI - Vaccination 4 date</v>
+        <v>AEFI - Sore throat</v>
       </c>
     </row>
     <row r="130">
@@ -4924,7 +4878,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B130" s="4" t="str">
-        <v>AEFI - Investigation needed</v>
+        <v>AEFI - Other (Severe event)</v>
       </c>
     </row>
     <row r="131">
@@ -4932,7 +4886,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B131" s="5" t="str">
-        <v>AEFI - Other diluent 4 name</v>
+        <v>AEFI - Other AEFI Date</v>
       </c>
     </row>
     <row r="132">
@@ -4940,7 +4894,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B132" s="4" t="str">
-        <v>AEFI - Reporter's address</v>
+        <v>AEFI - Loss of apetite</v>
       </c>
     </row>
     <row r="133">
@@ -4948,7 +4902,7 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B133" s="5" t="str">
-        <v>AEFI - Batch/lot number (Vaccine 1)</v>
+        <v>AEFI - Drowsiness</v>
       </c>
     </row>
     <row r="134">
@@ -4956,23 +4910,23 @@
         <v>AEFI - Adverse Events</v>
       </c>
       <c r="B134" s="4" t="str">
-        <v>AEFI - Fever</v>
+        <v>AEFI - Cough</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="5" t="str">
-        <v>AEFI - Adverse Events</v>
+        <v>Immunization tracker AEFI</v>
       </c>
       <c r="B135" s="5" t="str">
-        <v>AEFI - Batch/lot number (Vaccine 2)</v>
+        <v>AEFI - Batch/lot number (Vaccine 1)</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="4" t="str">
-        <v>AEFI - Adverse Events</v>
+        <v>Immunization tracker AEFI</v>
       </c>
       <c r="B136" s="4" t="str">
-        <v>AEFI - Seizure type</v>
+        <v>AEFI - Vaccination 1 date</v>
       </c>
     </row>
     <row r="137">
@@ -4980,7 +4934,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B137" s="5" t="str">
-        <v>AEFI - Vaccination 1 date</v>
+        <v>AEFI - Position/Department</v>
       </c>
     </row>
     <row r="138">
@@ -4988,7 +4942,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B138" s="4" t="str">
-        <v>AEFI - Batch/lot number (Vaccine 1)</v>
+        <v>AEFI - Expiry date (Diluent 1)</v>
       </c>
     </row>
     <row r="139">
@@ -4996,7 +4950,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B139" s="5" t="str">
-        <v>AEFI - Position/Department</v>
+        <v>AEFI - Reporter of AEFI case</v>
       </c>
     </row>
     <row r="140">
@@ -5004,7 +4958,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B140" s="4" t="str">
-        <v>AEFI - Expiry date (Diluent 1)</v>
+        <v>AEFI - Expiry date (Vaccine 1)</v>
       </c>
     </row>
     <row r="141">
@@ -5012,7 +4966,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B141" s="5" t="str">
-        <v>AEFI - Reporter of AEFI case</v>
+        <v>AEFI - Reporter's address</v>
       </c>
     </row>
     <row r="142">
@@ -5020,7 +4974,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B142" s="4" t="str">
-        <v>AEFI - Expiry date (Vaccine 1)</v>
+        <v>AEFI - Death</v>
       </c>
     </row>
     <row r="143">
@@ -5028,7 +4982,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B143" s="5" t="str">
-        <v>AEFI - Reporter's address</v>
+        <v>AEFI - Diluent batch/lot number 1</v>
       </c>
     </row>
     <row r="144">
@@ -5036,7 +4990,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B144" s="4" t="str">
-        <v>AEFI - Death</v>
+        <v>AEFI - Vaccine 1 name</v>
       </c>
     </row>
     <row r="145">
@@ -5044,7 +4998,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B145" s="5" t="str">
-        <v>AEFI - Diluent batch/lot number 1</v>
+        <v>AEFI - AEFI outcome</v>
       </c>
     </row>
     <row r="146">
@@ -5052,7 +5006,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B146" s="4" t="str">
-        <v>AEFI - Vaccine 1 name</v>
+        <v>AEFI - Reconstitution time 1</v>
       </c>
     </row>
     <row r="147">
@@ -5060,7 +5014,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B147" s="5" t="str">
-        <v>AEFI - AEFI outcome</v>
+        <v>AEFI - AEFI time</v>
       </c>
     </row>
     <row r="148">
@@ -5068,7 +5022,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B148" s="4" t="str">
-        <v>AEFI - Reconstitution time 1</v>
+        <v>AEFI - Contact number</v>
       </c>
     </row>
     <row r="149">
@@ -5076,7 +5030,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B149" s="5" t="str">
-        <v>AEFI - AEFI time</v>
+        <v>AEFI - E-mail address</v>
       </c>
     </row>
     <row r="150">
@@ -5084,7 +5038,7 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B150" s="4" t="str">
-        <v>AEFI - Contact number</v>
+        <v>AEFI - Medical history</v>
       </c>
     </row>
     <row r="151">
@@ -5092,22 +5046,6 @@
         <v>Immunization tracker AEFI</v>
       </c>
       <c r="B151" s="5" t="str">
-        <v>AEFI - E-mail address</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="4" t="str">
-        <v>Immunization tracker AEFI</v>
-      </c>
-      <c r="B152" s="4" t="str">
-        <v>AEFI - Medical history</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="5" t="str">
-        <v>Immunization tracker AEFI</v>
-      </c>
-      <c r="B153" s="5" t="str">
         <v>AEFI - Severe event reported</v>
       </c>
     </row>
@@ -5343,7 +5281,7 @@
         <v>Final Sub-classification</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>C. Coincidental Underlying or emerging condition(s), or condition(s) caused by exposure to something other than vaccine; C. Coincidental</v>
+        <v>C. Coincidental</v>
       </c>
     </row>
     <row r="4">
@@ -5554,13 +5492,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="121.7109375" customWidth="1"/>
+    <col min="2" max="2" width="98.7109375" customWidth="1"/>
     <col min="3" max="3" width="123.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
@@ -7298,23 +7236,6 @@
       </c>
       <c r="E102" s="4" t="str">
         <v>kvgPHkIUf2e</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="5" t="str">
-        <v>DDLVcciukAS</v>
-      </c>
-      <c r="B103" s="5" t="str">
-        <v>C. Coincidental Underlying or emerging condition(s), or condition(s) caused by exposure to something other than vaccine</v>
-      </c>
-      <c r="C103" s="5" t="str">
-        <v>Coincidental Underlying or emerging condition (s) caused by exposure to something other than vaccine</v>
-      </c>
-      <c r="D103" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E103" s="5" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -9661,13 +9582,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="174.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
@@ -9709,10 +9630,10 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Mobile phone number</v>
+        <v>Date of birth</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v/>
+        <v>patinfo_ageonsetunit</v>
       </c>
       <c r="C3" s="5" t="str">
         <v/>
@@ -9721,15 +9642,15 @@
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>fctSQp5nAYl</v>
+        <v>NI0QRzJvQ0k</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>National ID</v>
+        <v>First Name</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v/>
+        <v>first_name</v>
       </c>
       <c r="C4" s="4" t="str">
         <v/>
@@ -9738,23 +9659,108 @@
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>Ewi7FUfcHAD</v>
+        <v>sB1IHYu2xQT</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
+        <v>Home Address</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>patinfo_resadmin0</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>Xhdn49gUd52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>Mobile phone number</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C6" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D6" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E6" s="4" t="str">
+        <v>fctSQp5nAYl</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="str">
+        <v>National ID</v>
+      </c>
+      <c r="B7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="C7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>Ewi7FUfcHAD</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Sex</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>patinfo_sex</v>
+      </c>
+      <c r="C8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v>oindugucx72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>Surname</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v>surname</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <v>The patient's surname (family name)</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>ENRjVGxVL6l</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="str">
         <v>Unique System Identifier (EPI)</v>
       </c>
-      <c r="B5" s="5" t="str">
-        <v/>
-      </c>
-      <c r="C5" s="5" t="str">
+      <c r="B10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C10" s="4" t="str">
         <v>System-generated unique ID following pattern: EPI prefix + value randomly generated (#####) - Customize the length depending on the target population of your implementation</v>
       </c>
-      <c r="D5" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E5" s="5" t="str">
+      <c r="D10" s="4" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="4" t="str">
         <v>KSr2yTdu1AI</v>
       </c>
     </row>
@@ -9797,7 +9803,7 @@
         <v>Person</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-02-24</v>
+        <v>2021-03-19</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>EZkN8vYZwjR</v>

</xml_diff>